<commit_message>
Fixed custom plots (the way OF is used was very badly wrong @_@).  Added some custom fields for useful quantities in NKF1 and NKF6, PSC.
</commit_message>
<xml_diff>
--- a/CustomPlots/rate_tuning.xlsx
+++ b/CustomPlots/rate_tuning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\Documents\kVIS3_bsp_ardupilot\CustomPlots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D29CE8-C4E2-48C5-A1C1-8D4AA1B7AB63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5B7F87-276F-40B0-A7F1-24FFA95A4007}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{BA9E8F30-6C98-CF4B-8E95-183011E815A3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="52">
   <si>
     <t>KSID Custom Plot Definition</t>
   </si>
@@ -175,6 +175,18 @@
   </si>
   <si>
     <t>RateTuning</t>
+  </si>
+  <si>
+    <t>OF/bodyX</t>
+  </si>
+  <si>
+    <t>OF/bodyY</t>
+  </si>
+  <si>
+    <t>Roll Rate (OF)</t>
+  </si>
+  <si>
+    <t>Pitch Rate (OF)</t>
   </si>
 </sst>
 </file>
@@ -538,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7D595D-48C5-5044-8E94-F6ADF0970571}">
-  <dimension ref="A1:S13"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -701,13 +713,13 @@
         <v>24</v>
       </c>
       <c r="K7" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="O7">
-        <v>1</v>
+        <v>57.7</v>
       </c>
       <c r="R7" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="S7" t="s">
         <v>31</v>
@@ -715,7 +727,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -730,19 +742,19 @@
         <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G8" t="s">
         <v>24</v>
       </c>
       <c r="K8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O8">
         <v>1</v>
       </c>
       <c r="R8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S8" t="s">
         <v>31</v>
@@ -771,13 +783,13 @@
         <v>24</v>
       </c>
       <c r="K9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O9">
         <v>1</v>
       </c>
       <c r="R9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S9" t="s">
         <v>31</v>
@@ -785,13 +797,13 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>18</v>
@@ -800,19 +812,19 @@
         <v>23</v>
       </c>
       <c r="F10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G10" t="s">
         <v>24</v>
       </c>
       <c r="K10" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="O10">
-        <v>1</v>
+        <v>57.7</v>
       </c>
       <c r="R10" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="S10" t="s">
         <v>31</v>
@@ -820,13 +832,13 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>18</v>
@@ -835,19 +847,19 @@
         <v>23</v>
       </c>
       <c r="F11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G11" t="s">
         <v>24</v>
       </c>
       <c r="K11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O11">
         <v>1</v>
       </c>
       <c r="R11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="S11" t="s">
         <v>31</v>
@@ -855,7 +867,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -870,27 +882,27 @@
         <v>23</v>
       </c>
       <c r="F12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G12" t="s">
         <v>24</v>
       </c>
       <c r="K12" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="O12">
         <v>1</v>
       </c>
       <c r="R12" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="S12" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -905,21 +917,91 @@
         <v>23</v>
       </c>
       <c r="F13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G13" t="s">
         <v>24</v>
       </c>
       <c r="K13" t="s">
+        <v>37</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="R13" t="s">
+        <v>30</v>
+      </c>
+      <c r="S13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" t="s">
+        <v>42</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="R14" t="s">
+        <v>44</v>
+      </c>
+      <c r="S14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" t="s">
+        <v>24</v>
+      </c>
+      <c r="K15" t="s">
         <v>43</v>
       </c>
-      <c r="O13">
-        <v>1</v>
-      </c>
-      <c r="R13" t="s">
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="R15" t="s">
         <v>45</v>
       </c>
-      <c r="S13" t="s">
+      <c r="S15" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>